<commit_message>
Separated reference/consensus and locus data
</commit_message>
<xml_diff>
--- a/tabular/eve/ecv-ncbi-refseqs-side-data.xlsx
+++ b/tabular/eve/ecv-ncbi-refseqs-side-data.xlsx
@@ -1,34 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/eve/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4227E3-5C56-DF4C-A870-C52B22FF2B80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="1580" windowWidth="36380" windowHeight="20160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="3800" windowWidth="36380" windowHeight="20160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
   <si>
     <t>Circovirus</t>
   </si>
@@ -178,12 +172,33 @@
   </si>
   <si>
     <t>Endogenous circoviral element cress.8-tropileilaps consensus sequence</t>
+  </si>
+  <si>
+    <t>host_group_taxlevel</t>
+  </si>
+  <si>
+    <t>host_group_name</t>
+  </si>
+  <si>
+    <t>host_group_common_name</t>
+  </si>
+  <si>
+    <t>num_copies</t>
+  </si>
+  <si>
+    <t>locus_id</t>
+  </si>
+  <si>
+    <t>reftype</t>
+  </si>
+  <si>
+    <t>Consensus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -261,7 +276,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="316">
+  <cellStyleXfs count="326">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -461,6 +476,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -585,7 +610,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="316">
+  <cellStyles count="326">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -748,6 +773,11 @@
     <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -901,6 +931,11 @@
     <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="312" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="314" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="316" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="318" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1237,273 +1272,531 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="A1:F14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="41.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="35" style="2" customWidth="1"/>
-    <col min="3" max="3" width="63" style="2" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="15.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35" style="2" customWidth="1"/>
+    <col min="4" max="4" width="63" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Expanded ECV reference set
</commit_message>
<xml_diff>
--- a/tabular/eve/ecv-ncbi-refseqs-side-data.xlsx
+++ b/tabular/eve/ecv-ncbi-refseqs-side-data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="77">
   <si>
     <t>Circovirus</t>
   </si>
@@ -193,6 +193,66 @@
   </si>
   <si>
     <t>Consensus</t>
+  </si>
+  <si>
+    <t>REF_ECV_Galeopterus</t>
+  </si>
+  <si>
+    <t>REF_ECV_Chrysochloris</t>
+  </si>
+  <si>
+    <t>ecv-circo.13-galeopterus-con</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.13-galeopterus consensus sequence</t>
+  </si>
+  <si>
+    <t>ecv-circo.12-chrysochloris-con</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.12-chrysochloris consensus sequence</t>
+  </si>
+  <si>
+    <t>numeric_id</t>
+  </si>
+  <si>
+    <t>ecv-circo.3-mus_caroli</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>REF_ECV_Mus</t>
+  </si>
+  <si>
+    <t>REF_ECV_Monodelphis</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.4-monodelphis domestica reference sequence</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.3-mus_caroli reference sequence</t>
+  </si>
+  <si>
+    <t>ecv-circo.4-monodelphis_domestica</t>
+  </si>
+  <si>
+    <t>ecv-circo.8-kryptolebias-con</t>
+  </si>
+  <si>
+    <t>REF_ECV_Kryptolebias</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.8-kryptolebias consensus sequence</t>
+  </si>
+  <si>
+    <t>ecv-circo.6-cyprinus-con</t>
+  </si>
+  <si>
+    <t>REF_ECV_Cyprinus</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.6-cyprinus consensus sequence</t>
   </si>
 </sst>
 </file>
@@ -276,7 +336,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="326">
+  <cellStyleXfs count="386">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -476,6 +536,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -610,7 +730,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="326">
+  <cellStyles count="386">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -778,6 +898,36 @@
     <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="343" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="345" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="347" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="349" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="351" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="361" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -936,6 +1086,36 @@
     <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="342" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="348" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="350" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="352" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="354" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="356" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="358" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="360" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="362" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="372" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="376" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="378" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="380" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="382" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1273,28 +1453,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B13" sqref="A1:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="37.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="35" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63" style="2" customWidth="1"/>
+    <col min="4" max="4" width="85.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.1640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="22.1640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="7" max="8" width="9.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1317,33 +1497,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>10</v>
@@ -1351,7 +1534,10 @@
       <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="2">
+      <c r="G2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
         <v>1</v>
       </c>
       <c r="I2" s="2">
@@ -1366,19 +1552,22 @@
       <c r="L2" s="2">
         <v>1</v>
       </c>
+      <c r="M2" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>10</v>
@@ -1386,34 +1575,38 @@
       <c r="F3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>10</v>
@@ -1421,37 +1614,38 @@
       <c r="F4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>10</v>
@@ -1459,34 +1653,38 @@
       <c r="F5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>10</v>
@@ -1494,244 +1692,272 @@
       <c r="F6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1</v>
-      </c>
-      <c r="L6" s="2">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3">
         <v>6</v>
       </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1</v>
-      </c>
-      <c r="L7" s="2">
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3">
         <v>7</v>
       </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1</v>
-      </c>
-      <c r="L8" s="2">
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2">
-        <v>1</v>
-      </c>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1</v>
-      </c>
-      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3">
+        <v>8</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
-      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3">
+        <v>11</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2">
-        <v>1</v>
-      </c>
-      <c r="J11" s="2">
-        <v>1</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
-      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3">
+        <v>12</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1</v>
+      </c>
+      <c r="M11" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="2">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2">
-        <v>1</v>
-      </c>
-      <c r="J12" s="2">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
-      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3">
+        <v>13</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1</v>
+      </c>
+      <c r="M12" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>10</v>
@@ -1739,34 +1965,38 @@
       <c r="F13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="2">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2">
-        <v>1</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2">
-        <v>1</v>
-      </c>
-      <c r="L13" s="2">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>10</v>
@@ -1774,31 +2004,273 @@
       <c r="F14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2">
-        <v>1</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3">
+        <v>1</v>
+      </c>
+      <c r="M14" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+    <row r="15" spans="1:13">
+      <c r="A15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3">
+        <v>3</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+    <row r="16" spans="1:13">
+      <c r="A16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3">
+        <v>5</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3">
+        <v>1</v>
+      </c>
+      <c r="M16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3">
+        <v>6</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3">
+        <v>7</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3">
+        <v>8</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3">
+        <v>1</v>
+      </c>
+      <c r="M19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1</v>
+      </c>
+      <c r="K20" s="3">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
     </row>
   </sheetData>
+  <sortState ref="A2:M17">
+    <sortCondition ref="F2:F17"/>
+    <sortCondition ref="H2:H17"/>
+  </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>